<commit_message>
fixed mail and add/remove product
</commit_message>
<xml_diff>
--- a/Producten toevoegen.xlsx
+++ b/Producten toevoegen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lander Wuyts\IT\Sys Eng Projectweek\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD836537-B21A-4ADE-B054-E59F1931B8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5F12F7-7EED-4694-9DD5-01F9C7274EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2148" yWindow="2484" windowWidth="11520" windowHeight="8976" xr2:uid="{5239CB96-FA84-43C4-98A1-2144099ABCCF}"/>
   </bookViews>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8315AB79-82FD-4F9F-8156-629013D4B21E}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,73 +444,62 @@
         <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>44608</v>
+        <v>44592</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
-        <v>5414150631147</v>
+        <v>7610700949085</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>43496</v>
+        <v>44593</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <v>7610700949085</v>
+        <v>3502110008091</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2">
-        <v>44593</v>
+        <v>44592</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
-        <v>3502110008091</v>
+        <v>5410013110002</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
-        <v>44776</v>
+        <v>44593</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
-        <v>5410013110002</v>
+        <v>5411028070480</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2">
-        <v>44596</v>
+        <v>44592</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <v>5411028070480</v>
+        <v>5411188115472</v>
       </c>
       <c r="B7">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C7" s="2">
         <v>44592</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>5411188115472</v>
-      </c>
-      <c r="B8">
-        <v>63</v>
-      </c>
-      <c r="C8" s="2">
-        <v>44589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed minor issue with removing products
</commit_message>
<xml_diff>
--- a/Producten toevoegen.xlsx
+++ b/Producten toevoegen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lander Wuyts\IT\Sys Eng Projectweek\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5F12F7-7EED-4694-9DD5-01F9C7274EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA01512-433B-4946-99B0-3A5135E0DE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2148" yWindow="2484" windowWidth="11520" windowHeight="8976" xr2:uid="{5239CB96-FA84-43C4-98A1-2144099ABCCF}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,7 +441,7 @@
         <v>7610700949085</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <v>44592</v>
@@ -452,7 +452,7 @@
         <v>7610700949085</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>44593</v>
@@ -463,7 +463,7 @@
         <v>3502110008091</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>44592</v>
@@ -474,7 +474,7 @@
         <v>5410013110002</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
         <v>44593</v>
@@ -485,7 +485,7 @@
         <v>5411028070480</v>
       </c>
       <c r="B6">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
         <v>44592</v>
@@ -496,7 +496,7 @@
         <v>5411188115472</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2">
         <v>44592</v>

</xml_diff>